<commit_message>
- Fixed update image
</commit_message>
<xml_diff>
--- a/Document/Bug.xlsx
+++ b/Document/Bug.xlsx
@@ -42,7 +42,7 @@
     <t>Enter user name then choose edit apartment. Notice can't change image.</t>
   </si>
   <si>
-    <t>Open</t>
+    <t>Fixed</t>
   </si>
 </sst>
 </file>
@@ -370,7 +370,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -403,7 +403,7 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>